<commit_message>
Implement export to html
</commit_message>
<xml_diff>
--- a/src/main/resources/Automatic_and_systems.xlsx
+++ b/src/main/resources/Automatic_and_systems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.frishbuter/IdeaProjects/CourseTimeTable/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD01A3AB-71E5-2647-A207-801D3D9FF6BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9605FE-9BE8-D14B-BC8A-208721CFF6BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32780" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="8080" windowWidth="32860" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Преподаватели" sheetId="13" r:id="rId1"/>
@@ -1031,6 +1031,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1039,10 +1043,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1327,7 +1327,7 @@
   <dimension ref="A1:G478"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="15"/>
@@ -1341,19 +1341,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="12" customHeight="1">
-      <c r="A1" s="14"/>
+      <c r="A1" s="10"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="13"/>
+      <c r="A2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="16">
-      <c r="A3" s="13"/>
+      <c r="A3" s="11"/>
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="13"/>
+      <c r="A4" s="11"/>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="4"/>
@@ -1412,7 +1412,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="11"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>21</v>
@@ -1429,7 +1429,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="11"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
@@ -1448,7 +1448,7 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="16" thickBot="1">
-      <c r="A12" s="12"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>21</v>
@@ -1465,7 +1465,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="4"/>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="6" t="s">
         <v>28</v>
       </c>
@@ -1501,7 +1501,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="6" t="s">
         <v>25</v>
       </c>
@@ -1520,7 +1520,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" thickBot="1">
-      <c r="A16" s="12"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
         <v>9</v>
@@ -1535,7 +1535,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="4"/>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="6" t="s">
         <v>9</v>
       </c>
@@ -1573,7 +1573,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="11"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="7" t="s">
         <v>37</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="16" thickBot="1">
-      <c r="A20" s="12"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="6" t="s">
         <v>33</v>
       </c>
@@ -1605,7 +1605,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="4"/>
@@ -1620,7 +1620,7 @@
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
         <v>25</v>
@@ -1635,7 +1635,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="6" t="s">
         <v>9</v>
       </c>
@@ -1652,7 +1652,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" thickBot="1">
-      <c r="A24" s="12"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
         <v>9</v>
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="4"/>
@@ -1678,7 +1678,7 @@
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
         <v>9</v>
@@ -1691,7 +1691,7 @@
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="11"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="6" t="s">
         <v>9</v>
       </c>
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="16" thickBot="1">
-      <c r="A28" s="12"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8" t="s">
         <v>29</v>
@@ -1730,19 +1730,19 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="13"/>
+      <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="13"/>
+      <c r="A34" s="11"/>
     </row>
     <row r="35" spans="1:7" ht="16">
-      <c r="A35" s="13"/>
+      <c r="A35" s="11"/>
       <c r="D35" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="13"/>
+      <c r="A36" s="11"/>
     </row>
     <row r="37" spans="1:7">
       <c r="B37" t="s">
@@ -1784,7 +1784,7 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B41" s="4"/>
@@ -1801,7 +1801,7 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="11"/>
+      <c r="A42" s="13"/>
       <c r="B42" s="6" t="s">
         <v>9</v>
       </c>
@@ -1818,7 +1818,7 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="11"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="7" t="s">
         <v>47</v>
       </c>
@@ -1835,7 +1835,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="16" thickBot="1">
-      <c r="A44" s="12"/>
+      <c r="A44" s="14"/>
       <c r="B44" s="6" t="s">
         <v>45</v>
       </c>
@@ -1852,7 +1852,7 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -1869,7 +1869,7 @@
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="11"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="6" t="s">
         <v>53</v>
       </c>
@@ -1886,7 +1886,7 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="11"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="7" t="s">
         <v>43</v>
       </c>
@@ -1907,7 +1907,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="16" thickBot="1">
-      <c r="A48" s="12"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="6" t="s">
         <v>46</v>
       </c>
@@ -1924,7 +1924,7 @@
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -1939,7 +1939,7 @@
       <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="11"/>
+      <c r="A50" s="13"/>
       <c r="B50" s="6" t="s">
         <v>53</v>
       </c>
@@ -1952,7 +1952,7 @@
       <c r="G50" s="6"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="11"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7" t="s">
         <v>59</v>
@@ -1971,7 +1971,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="16" thickBot="1">
-      <c r="A52" s="12"/>
+      <c r="A52" s="14"/>
       <c r="B52" s="6" t="s">
         <v>9</v>
       </c>
@@ -1984,7 +1984,7 @@
       <c r="G52" s="6"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="4"/>
@@ -1997,7 +1997,7 @@
       <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="11"/>
+      <c r="A54" s="13"/>
       <c r="B54" s="6" t="s">
         <v>9</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="G54" s="6"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="11"/>
+      <c r="A55" s="13"/>
       <c r="B55" s="7" t="s">
         <v>61</v>
       </c>
@@ -2031,7 +2031,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="16" thickBot="1">
-      <c r="A56" s="12"/>
+      <c r="A56" s="14"/>
       <c r="B56" s="6" t="s">
         <v>62</v>
       </c>
@@ -2046,7 +2046,7 @@
       <c r="G56" s="6"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -2059,7 +2059,7 @@
       <c r="G57" s="4"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="11"/>
+      <c r="A58" s="13"/>
       <c r="B58" s="6" t="s">
         <v>62</v>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="G58" s="6"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="11"/>
+      <c r="A59" s="13"/>
       <c r="B59" s="7"/>
       <c r="C59" s="6" t="s">
         <v>9</v>
@@ -2091,7 +2091,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="16" thickBot="1">
-      <c r="A60" s="12"/>
+      <c r="A60" s="14"/>
       <c r="B60" s="8" t="s">
         <v>9</v>
       </c>
@@ -2109,19 +2109,19 @@
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="13"/>
+      <c r="A65" s="11"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="13"/>
+      <c r="A66" s="11"/>
     </row>
     <row r="67" spans="1:7" ht="16">
-      <c r="A67" s="13"/>
+      <c r="A67" s="11"/>
       <c r="D67" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="13"/>
+      <c r="A68" s="11"/>
     </row>
     <row r="69" spans="1:7">
       <c r="B69" t="s">
@@ -2163,7 +2163,7 @@
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B73" s="4"/>
@@ -2176,7 +2176,7 @@
       <c r="G73" s="4"/>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="11"/>
+      <c r="A74" s="13"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6" t="s">
@@ -2193,7 +2193,7 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="11"/>
+      <c r="A75" s="13"/>
       <c r="B75" s="6" t="s">
         <v>9</v>
       </c>
@@ -2214,7 +2214,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="16" thickBot="1">
-      <c r="A76" s="12"/>
+      <c r="A76" s="14"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6" t="s">
@@ -2231,7 +2231,7 @@
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="10" t="s">
+      <c r="A77" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B77" s="4"/>
@@ -2244,7 +2244,7 @@
       <c r="G77" s="4"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="11"/>
+      <c r="A78" s="13"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6" t="s">
@@ -2257,7 +2257,7 @@
       <c r="G78" s="6"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="11"/>
+      <c r="A79" s="13"/>
       <c r="B79" s="6" t="s">
         <v>9</v>
       </c>
@@ -2276,7 +2276,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="16" thickBot="1">
-      <c r="A80" s="12"/>
+      <c r="A80" s="14"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6" t="s">
@@ -2289,7 +2289,7 @@
       <c r="G80" s="6"/>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="10" t="s">
+      <c r="A81" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B81" s="4"/>
@@ -2304,7 +2304,7 @@
       <c r="G81" s="4"/>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="11"/>
+      <c r="A82" s="13"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6" t="s">
@@ -2319,7 +2319,7 @@
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="11"/>
+      <c r="A83" s="13"/>
       <c r="B83" s="6" t="s">
         <v>9</v>
       </c>
@@ -2338,7 +2338,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" ht="16" thickBot="1">
-      <c r="A84" s="12"/>
+      <c r="A84" s="14"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6" t="s">
@@ -2353,7 +2353,7 @@
       </c>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B85" s="4"/>
@@ -2366,7 +2366,7 @@
       <c r="G85" s="4"/>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="11"/>
+      <c r="A86" s="13"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
@@ -2377,7 +2377,7 @@
       <c r="G86" s="6"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="11"/>
+      <c r="A87" s="13"/>
       <c r="B87" s="6" t="s">
         <v>9</v>
       </c>
@@ -2398,7 +2398,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="16" thickBot="1">
-      <c r="A88" s="12"/>
+      <c r="A88" s="14"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
@@ -2409,7 +2409,7 @@
       <c r="G88" s="6"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="10" t="s">
+      <c r="A89" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B89" s="4"/>
@@ -2420,7 +2420,7 @@
       <c r="G89" s="4"/>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="11"/>
+      <c r="A90" s="13"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
@@ -2429,7 +2429,7 @@
       <c r="G90" s="6"/>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="11"/>
+      <c r="A91" s="13"/>
       <c r="B91" s="6" t="s">
         <v>9</v>
       </c>
@@ -2450,7 +2450,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="16" thickBot="1">
-      <c r="A92" s="12"/>
+      <c r="A92" s="14"/>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
@@ -2464,19 +2464,19 @@
       </c>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="13"/>
+      <c r="A97" s="11"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="13"/>
+      <c r="A98" s="11"/>
     </row>
     <row r="99" spans="1:7" ht="16">
-      <c r="A99" s="13"/>
+      <c r="A99" s="11"/>
       <c r="D99" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="13"/>
+      <c r="A100" s="11"/>
     </row>
     <row r="101" spans="1:7">
       <c r="B101" t="s">
@@ -2518,7 +2518,7 @@
       </c>
     </row>
     <row r="105" spans="1:7">
-      <c r="A105" s="10" t="s">
+      <c r="A105" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B105" s="4"/>
@@ -2529,7 +2529,7 @@
       <c r="G105" s="4"/>
     </row>
     <row r="106" spans="1:7">
-      <c r="A106" s="11"/>
+      <c r="A106" s="13"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
@@ -2538,7 +2538,7 @@
       <c r="G106" s="6"/>
     </row>
     <row r="107" spans="1:7">
-      <c r="A107" s="11"/>
+      <c r="A107" s="13"/>
       <c r="B107" s="6" t="s">
         <v>9</v>
       </c>
@@ -2559,7 +2559,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="16" thickBot="1">
-      <c r="A108" s="12"/>
+      <c r="A108" s="14"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
@@ -2568,7 +2568,7 @@
       <c r="G108" s="6"/>
     </row>
     <row r="109" spans="1:7">
-      <c r="A109" s="10" t="s">
+      <c r="A109" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B109" s="4"/>
@@ -2579,7 +2579,7 @@
       <c r="G109" s="4"/>
     </row>
     <row r="110" spans="1:7">
-      <c r="A110" s="11"/>
+      <c r="A110" s="13"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
@@ -2588,7 +2588,7 @@
       <c r="G110" s="6"/>
     </row>
     <row r="111" spans="1:7">
-      <c r="A111" s="11"/>
+      <c r="A111" s="13"/>
       <c r="B111" s="6" t="s">
         <v>9</v>
       </c>
@@ -2609,7 +2609,7 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="16" thickBot="1">
-      <c r="A112" s="12"/>
+      <c r="A112" s="14"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
@@ -2618,7 +2618,7 @@
       <c r="G112" s="6"/>
     </row>
     <row r="113" spans="1:7">
-      <c r="A113" s="10" t="s">
+      <c r="A113" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B113" s="4"/>
@@ -2629,7 +2629,7 @@
       <c r="G113" s="4"/>
     </row>
     <row r="114" spans="1:7">
-      <c r="A114" s="11"/>
+      <c r="A114" s="13"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
@@ -2638,7 +2638,7 @@
       <c r="G114" s="6"/>
     </row>
     <row r="115" spans="1:7">
-      <c r="A115" s="11"/>
+      <c r="A115" s="13"/>
       <c r="B115" s="6" t="s">
         <v>9</v>
       </c>
@@ -2659,7 +2659,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="16" thickBot="1">
-      <c r="A116" s="12"/>
+      <c r="A116" s="14"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
@@ -2668,7 +2668,7 @@
       <c r="G116" s="6"/>
     </row>
     <row r="117" spans="1:7">
-      <c r="A117" s="10" t="s">
+      <c r="A117" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B117" s="4"/>
@@ -2679,7 +2679,7 @@
       <c r="G117" s="4"/>
     </row>
     <row r="118" spans="1:7">
-      <c r="A118" s="11"/>
+      <c r="A118" s="13"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6" t="s">
         <v>78</v>
@@ -2690,7 +2690,7 @@
       <c r="G118" s="6"/>
     </row>
     <row r="119" spans="1:7">
-      <c r="A119" s="11"/>
+      <c r="A119" s="13"/>
       <c r="B119" s="6" t="s">
         <v>9</v>
       </c>
@@ -2711,7 +2711,7 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="16" thickBot="1">
-      <c r="A120" s="12"/>
+      <c r="A120" s="14"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
@@ -2720,7 +2720,7 @@
       <c r="G120" s="6"/>
     </row>
     <row r="121" spans="1:7">
-      <c r="A121" s="10" t="s">
+      <c r="A121" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B121" s="4"/>
@@ -2731,7 +2731,7 @@
       <c r="G121" s="4"/>
     </row>
     <row r="122" spans="1:7">
-      <c r="A122" s="11"/>
+      <c r="A122" s="13"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
       <c r="D122" s="6"/>
@@ -2740,7 +2740,7 @@
       <c r="G122" s="6"/>
     </row>
     <row r="123" spans="1:7">
-      <c r="A123" s="11"/>
+      <c r="A123" s="13"/>
       <c r="B123" s="6" t="s">
         <v>9</v>
       </c>
@@ -2761,7 +2761,7 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="16" thickBot="1">
-      <c r="A124" s="12"/>
+      <c r="A124" s="14"/>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
@@ -2775,19 +2775,19 @@
       </c>
     </row>
     <row r="129" spans="1:7">
-      <c r="A129" s="13"/>
+      <c r="A129" s="11"/>
     </row>
     <row r="130" spans="1:7">
-      <c r="A130" s="13"/>
+      <c r="A130" s="11"/>
     </row>
     <row r="131" spans="1:7" ht="16">
-      <c r="A131" s="13"/>
+      <c r="A131" s="11"/>
       <c r="D131" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:7">
-      <c r="A132" s="13"/>
+      <c r="A132" s="11"/>
     </row>
     <row r="133" spans="1:7">
       <c r="B133" t="s">
@@ -2829,7 +2829,7 @@
       </c>
     </row>
     <row r="137" spans="1:7">
-      <c r="A137" s="10" t="s">
+      <c r="A137" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B137" s="4" t="s">
@@ -2842,7 +2842,7 @@
       <c r="G137" s="4"/>
     </row>
     <row r="138" spans="1:7">
-      <c r="A138" s="11"/>
+      <c r="A138" s="13"/>
       <c r="B138" s="6" t="s">
         <v>97</v>
       </c>
@@ -2859,7 +2859,7 @@
       </c>
     </row>
     <row r="139" spans="1:7">
-      <c r="A139" s="11"/>
+      <c r="A139" s="13"/>
       <c r="B139" s="7"/>
       <c r="C139" s="6" t="s">
         <v>9</v>
@@ -2878,7 +2878,7 @@
       </c>
     </row>
     <row r="140" spans="1:7" ht="16" thickBot="1">
-      <c r="A140" s="12"/>
+      <c r="A140" s="14"/>
       <c r="B140" s="6" t="s">
         <v>9</v>
       </c>
@@ -2893,7 +2893,7 @@
       <c r="G140" s="6"/>
     </row>
     <row r="141" spans="1:7">
-      <c r="A141" s="10" t="s">
+      <c r="A141" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B141" s="4" t="s">
@@ -2914,7 +2914,7 @@
       </c>
     </row>
     <row r="142" spans="1:7">
-      <c r="A142" s="11"/>
+      <c r="A142" s="13"/>
       <c r="B142" s="6" t="s">
         <v>97</v>
       </c>
@@ -2933,7 +2933,7 @@
       </c>
     </row>
     <row r="143" spans="1:7">
-      <c r="A143" s="11"/>
+      <c r="A143" s="13"/>
       <c r="B143" s="7"/>
       <c r="C143" s="6" t="s">
         <v>9</v>
@@ -2952,7 +2952,7 @@
       </c>
     </row>
     <row r="144" spans="1:7" ht="16" thickBot="1">
-      <c r="A144" s="12"/>
+      <c r="A144" s="14"/>
       <c r="B144" s="6" t="s">
         <v>9</v>
       </c>
@@ -2971,7 +2971,7 @@
       </c>
     </row>
     <row r="145" spans="1:7">
-      <c r="A145" s="10" t="s">
+      <c r="A145" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B145" s="4" t="s">
@@ -2992,7 +2992,7 @@
       </c>
     </row>
     <row r="146" spans="1:7">
-      <c r="A146" s="11"/>
+      <c r="A146" s="13"/>
       <c r="B146" s="6" t="s">
         <v>92</v>
       </c>
@@ -3013,7 +3013,7 @@
       </c>
     </row>
     <row r="147" spans="1:7">
-      <c r="A147" s="11"/>
+      <c r="A147" s="13"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7" t="s">
         <v>84</v>
@@ -3030,7 +3030,7 @@
       <c r="G147" s="7"/>
     </row>
     <row r="148" spans="1:7" ht="16" thickBot="1">
-      <c r="A148" s="12"/>
+      <c r="A148" s="14"/>
       <c r="B148" s="6" t="s">
         <v>9</v>
       </c>
@@ -3049,7 +3049,7 @@
       </c>
     </row>
     <row r="149" spans="1:7">
-      <c r="A149" s="10" t="s">
+      <c r="A149" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B149" s="4" t="s">
@@ -3066,7 +3066,7 @@
       <c r="G149" s="4"/>
     </row>
     <row r="150" spans="1:7">
-      <c r="A150" s="11"/>
+      <c r="A150" s="13"/>
       <c r="B150" s="6" t="s">
         <v>97</v>
       </c>
@@ -3083,7 +3083,7 @@
       <c r="G150" s="6"/>
     </row>
     <row r="151" spans="1:7">
-      <c r="A151" s="11"/>
+      <c r="A151" s="13"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7" t="s">
         <v>81</v>
@@ -3100,7 +3100,7 @@
       </c>
     </row>
     <row r="152" spans="1:7" ht="16" thickBot="1">
-      <c r="A152" s="12"/>
+      <c r="A152" s="14"/>
       <c r="B152" s="6" t="s">
         <v>9</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="G152" s="6"/>
     </row>
     <row r="153" spans="1:7">
-      <c r="A153" s="10" t="s">
+      <c r="A153" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B153" s="4"/>
@@ -3130,7 +3130,7 @@
       <c r="G153" s="4"/>
     </row>
     <row r="154" spans="1:7">
-      <c r="A154" s="11"/>
+      <c r="A154" s="13"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
       <c r="D154" s="6" t="s">
@@ -3141,7 +3141,7 @@
       <c r="G154" s="6"/>
     </row>
     <row r="155" spans="1:7">
-      <c r="A155" s="11"/>
+      <c r="A155" s="13"/>
       <c r="B155" s="6" t="s">
         <v>9</v>
       </c>
@@ -3162,7 +3162,7 @@
       </c>
     </row>
     <row r="156" spans="1:7" ht="16" thickBot="1">
-      <c r="A156" s="12"/>
+      <c r="A156" s="14"/>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8" t="s">
@@ -3178,19 +3178,19 @@
       </c>
     </row>
     <row r="161" spans="1:7">
-      <c r="A161" s="13"/>
+      <c r="A161" s="11"/>
     </row>
     <row r="162" spans="1:7">
-      <c r="A162" s="13"/>
+      <c r="A162" s="11"/>
     </row>
     <row r="163" spans="1:7" ht="16">
-      <c r="A163" s="13"/>
+      <c r="A163" s="11"/>
       <c r="D163" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:7">
-      <c r="A164" s="13"/>
+      <c r="A164" s="11"/>
     </row>
     <row r="165" spans="1:7">
       <c r="B165" t="s">
@@ -3232,7 +3232,7 @@
       </c>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="10" t="s">
+      <c r="A169" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B169" s="4"/>
@@ -3243,7 +3243,7 @@
       <c r="G169" s="4"/>
     </row>
     <row r="170" spans="1:7">
-      <c r="A170" s="11"/>
+      <c r="A170" s="13"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
       <c r="D170" s="6"/>
@@ -3252,7 +3252,7 @@
       <c r="G170" s="6"/>
     </row>
     <row r="171" spans="1:7">
-      <c r="A171" s="11"/>
+      <c r="A171" s="13"/>
       <c r="B171" s="6" t="s">
         <v>9</v>
       </c>
@@ -3273,7 +3273,7 @@
       </c>
     </row>
     <row r="172" spans="1:7" ht="16" thickBot="1">
-      <c r="A172" s="12"/>
+      <c r="A172" s="14"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
       <c r="D172" s="6"/>
@@ -3282,7 +3282,7 @@
       <c r="G172" s="6"/>
     </row>
     <row r="173" spans="1:7">
-      <c r="A173" s="10" t="s">
+      <c r="A173" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B173" s="4"/>
@@ -3293,7 +3293,7 @@
       <c r="G173" s="4"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="11"/>
+      <c r="A174" s="13"/>
       <c r="B174" s="6" t="s">
         <v>9</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="G174" s="6"/>
     </row>
     <row r="175" spans="1:7">
-      <c r="A175" s="11"/>
+      <c r="A175" s="13"/>
       <c r="B175" s="7" t="s">
         <v>103</v>
       </c>
@@ -3327,7 +3327,7 @@
       </c>
     </row>
     <row r="176" spans="1:7" ht="16" thickBot="1">
-      <c r="A176" s="12"/>
+      <c r="A176" s="14"/>
       <c r="B176" s="6" t="s">
         <v>105</v>
       </c>
@@ -3340,7 +3340,7 @@
       <c r="G176" s="6"/>
     </row>
     <row r="177" spans="1:7">
-      <c r="A177" s="10" t="s">
+      <c r="A177" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B177" s="4"/>
@@ -3357,7 +3357,7 @@
       <c r="G177" s="4"/>
     </row>
     <row r="178" spans="1:7">
-      <c r="A178" s="11"/>
+      <c r="A178" s="13"/>
       <c r="B178" s="6" t="s">
         <v>9</v>
       </c>
@@ -3374,7 +3374,7 @@
       <c r="G178" s="6"/>
     </row>
     <row r="179" spans="1:7">
-      <c r="A179" s="11"/>
+      <c r="A179" s="13"/>
       <c r="B179" s="7" t="s">
         <v>108</v>
       </c>
@@ -3389,7 +3389,7 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="16" thickBot="1">
-      <c r="A180" s="12"/>
+      <c r="A180" s="14"/>
       <c r="B180" s="6" t="s">
         <v>107</v>
       </c>
@@ -3406,7 +3406,7 @@
       <c r="G180" s="6"/>
     </row>
     <row r="181" spans="1:7">
-      <c r="A181" s="10" t="s">
+      <c r="A181" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B181" s="4"/>
@@ -3419,7 +3419,7 @@
       <c r="G181" s="4"/>
     </row>
     <row r="182" spans="1:7">
-      <c r="A182" s="11"/>
+      <c r="A182" s="13"/>
       <c r="B182" s="6"/>
       <c r="C182" s="6"/>
       <c r="D182" s="6"/>
@@ -3430,7 +3430,7 @@
       <c r="G182" s="6"/>
     </row>
     <row r="183" spans="1:7">
-      <c r="A183" s="11"/>
+      <c r="A183" s="13"/>
       <c r="B183" s="6" t="s">
         <v>9</v>
       </c>
@@ -3449,7 +3449,7 @@
       </c>
     </row>
     <row r="184" spans="1:7" ht="16" thickBot="1">
-      <c r="A184" s="12"/>
+      <c r="A184" s="14"/>
       <c r="B184" s="6"/>
       <c r="C184" s="6"/>
       <c r="D184" s="6"/>
@@ -3460,7 +3460,7 @@
       <c r="G184" s="6"/>
     </row>
     <row r="185" spans="1:7">
-      <c r="A185" s="10" t="s">
+      <c r="A185" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B185" s="4"/>
@@ -3471,7 +3471,7 @@
       <c r="G185" s="4"/>
     </row>
     <row r="186" spans="1:7">
-      <c r="A186" s="11"/>
+      <c r="A186" s="13"/>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
       <c r="D186" s="6"/>
@@ -3480,7 +3480,7 @@
       <c r="G186" s="6"/>
     </row>
     <row r="187" spans="1:7">
-      <c r="A187" s="11"/>
+      <c r="A187" s="13"/>
       <c r="B187" s="6" t="s">
         <v>9</v>
       </c>
@@ -3501,7 +3501,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="16" thickBot="1">
-      <c r="A188" s="12"/>
+      <c r="A188" s="14"/>
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
       <c r="D188" s="8"/>
@@ -3515,19 +3515,19 @@
       </c>
     </row>
     <row r="193" spans="1:7">
-      <c r="A193" s="13"/>
+      <c r="A193" s="11"/>
     </row>
     <row r="194" spans="1:7">
-      <c r="A194" s="13"/>
+      <c r="A194" s="11"/>
     </row>
     <row r="195" spans="1:7" ht="16">
-      <c r="A195" s="13"/>
+      <c r="A195" s="11"/>
       <c r="D195" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:7">
-      <c r="A196" s="13"/>
+      <c r="A196" s="11"/>
     </row>
     <row r="197" spans="1:7">
       <c r="B197" t="s">
@@ -3569,7 +3569,7 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="10" t="s">
+      <c r="A201" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B201" s="4"/>
@@ -3586,7 +3586,7 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="11"/>
+      <c r="A202" s="13"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="6"/>
@@ -3601,7 +3601,7 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="11"/>
+      <c r="A203" s="13"/>
       <c r="B203" s="6" t="s">
         <v>9</v>
       </c>
@@ -3616,7 +3616,7 @@
       <c r="G203" s="7"/>
     </row>
     <row r="204" spans="1:7" ht="16" thickBot="1">
-      <c r="A204" s="12"/>
+      <c r="A204" s="14"/>
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
       <c r="D204" s="6"/>
@@ -3631,7 +3631,7 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="10" t="s">
+      <c r="A205" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B205" s="4"/>
@@ -3648,7 +3648,7 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="11"/>
+      <c r="A206" s="13"/>
       <c r="B206" s="6"/>
       <c r="C206" s="6" t="s">
         <v>9</v>
@@ -3665,7 +3665,7 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="11"/>
+      <c r="A207" s="13"/>
       <c r="B207" s="6" t="s">
         <v>9</v>
       </c>
@@ -3682,7 +3682,7 @@
       <c r="G207" s="7"/>
     </row>
     <row r="208" spans="1:7" ht="16" thickBot="1">
-      <c r="A208" s="12"/>
+      <c r="A208" s="14"/>
       <c r="B208" s="6"/>
       <c r="C208" s="6" t="s">
         <v>123</v>
@@ -3699,7 +3699,7 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="10" t="s">
+      <c r="A209" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B209" s="4"/>
@@ -3712,7 +3712,7 @@
       <c r="G209" s="4"/>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="11"/>
+      <c r="A210" s="13"/>
       <c r="B210" s="6" t="s">
         <v>9</v>
       </c>
@@ -3729,7 +3729,7 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="11"/>
+      <c r="A211" s="13"/>
       <c r="B211" s="7" t="s">
         <v>111</v>
       </c>
@@ -3750,7 +3750,7 @@
       </c>
     </row>
     <row r="212" spans="1:7" ht="16" thickBot="1">
-      <c r="A212" s="12"/>
+      <c r="A212" s="14"/>
       <c r="B212" s="6" t="s">
         <v>115</v>
       </c>
@@ -3767,7 +3767,7 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="10" t="s">
+      <c r="A213" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B213" s="4" t="s">
@@ -3782,7 +3782,7 @@
       <c r="G213" s="4"/>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="11"/>
+      <c r="A214" s="13"/>
       <c r="B214" s="6" t="s">
         <v>126</v>
       </c>
@@ -3795,7 +3795,7 @@
       <c r="G214" s="6"/>
     </row>
     <row r="215" spans="1:7">
-      <c r="A215" s="11"/>
+      <c r="A215" s="13"/>
       <c r="B215" s="7"/>
       <c r="C215" s="6" t="s">
         <v>9</v>
@@ -3814,7 +3814,7 @@
       </c>
     </row>
     <row r="216" spans="1:7" ht="16" thickBot="1">
-      <c r="A216" s="12"/>
+      <c r="A216" s="14"/>
       <c r="B216" s="6" t="s">
         <v>9</v>
       </c>
@@ -3827,7 +3827,7 @@
       <c r="G216" s="6"/>
     </row>
     <row r="217" spans="1:7">
-      <c r="A217" s="10" t="s">
+      <c r="A217" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B217" s="4"/>
@@ -3838,7 +3838,7 @@
       <c r="G217" s="4"/>
     </row>
     <row r="218" spans="1:7">
-      <c r="A218" s="11"/>
+      <c r="A218" s="13"/>
       <c r="B218" s="6"/>
       <c r="C218" s="6"/>
       <c r="D218" s="6"/>
@@ -3847,7 +3847,7 @@
       <c r="G218" s="6"/>
     </row>
     <row r="219" spans="1:7">
-      <c r="A219" s="11"/>
+      <c r="A219" s="13"/>
       <c r="B219" s="6" t="s">
         <v>9</v>
       </c>
@@ -3868,7 +3868,7 @@
       </c>
     </row>
     <row r="220" spans="1:7" ht="16" thickBot="1">
-      <c r="A220" s="12"/>
+      <c r="A220" s="14"/>
       <c r="B220" s="8"/>
       <c r="C220" s="8"/>
       <c r="D220" s="8"/>
@@ -3882,19 +3882,19 @@
       </c>
     </row>
     <row r="225" spans="1:7">
-      <c r="A225" s="13"/>
+      <c r="A225" s="11"/>
     </row>
     <row r="226" spans="1:7">
-      <c r="A226" s="13"/>
+      <c r="A226" s="11"/>
     </row>
     <row r="227" spans="1:7" ht="16">
-      <c r="A227" s="13"/>
+      <c r="A227" s="11"/>
       <c r="D227" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="13"/>
+      <c r="A228" s="11"/>
     </row>
     <row r="229" spans="1:7">
       <c r="B229" t="s">
@@ -3936,7 +3936,7 @@
       </c>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="10" t="s">
+      <c r="A233" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B233" s="4"/>
@@ -3955,7 +3955,7 @@
       <c r="G233" s="4"/>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="11"/>
+      <c r="A234" s="13"/>
       <c r="B234" s="6"/>
       <c r="C234" s="6" t="s">
         <v>133</v>
@@ -3972,7 +3972,7 @@
       <c r="G234" s="6"/>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="11"/>
+      <c r="A235" s="13"/>
       <c r="B235" s="6" t="s">
         <v>9</v>
       </c>
@@ -3991,7 +3991,7 @@
       </c>
     </row>
     <row r="236" spans="1:7" ht="16" thickBot="1">
-      <c r="A236" s="12"/>
+      <c r="A236" s="14"/>
       <c r="B236" s="6"/>
       <c r="C236" s="6" t="s">
         <v>138</v>
@@ -4008,7 +4008,7 @@
       <c r="G236" s="6"/>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="10" t="s">
+      <c r="A237" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B237" s="4" t="s">
@@ -4029,7 +4029,7 @@
       </c>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="11"/>
+      <c r="A238" s="13"/>
       <c r="B238" s="6" t="s">
         <v>135</v>
       </c>
@@ -4048,7 +4048,7 @@
       </c>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="11"/>
+      <c r="A239" s="13"/>
       <c r="B239" s="7"/>
       <c r="C239" s="7"/>
       <c r="D239" s="7"/>
@@ -4061,7 +4061,7 @@
       <c r="G239" s="7"/>
     </row>
     <row r="240" spans="1:7" ht="16" thickBot="1">
-      <c r="A240" s="12"/>
+      <c r="A240" s="14"/>
       <c r="B240" s="6" t="s">
         <v>9</v>
       </c>
@@ -4080,7 +4080,7 @@
       </c>
     </row>
     <row r="241" spans="1:7">
-      <c r="A241" s="10" t="s">
+      <c r="A241" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B241" s="4"/>
@@ -4093,7 +4093,7 @@
       </c>
     </row>
     <row r="242" spans="1:7">
-      <c r="A242" s="11"/>
+      <c r="A242" s="13"/>
       <c r="B242" s="6" t="s">
         <v>9</v>
       </c>
@@ -4110,7 +4110,7 @@
       </c>
     </row>
     <row r="243" spans="1:7">
-      <c r="A243" s="11"/>
+      <c r="A243" s="13"/>
       <c r="B243" s="7" t="s">
         <v>43</v>
       </c>
@@ -4131,7 +4131,7 @@
       </c>
     </row>
     <row r="244" spans="1:7" ht="16" thickBot="1">
-      <c r="A244" s="12"/>
+      <c r="A244" s="14"/>
       <c r="B244" s="6" t="s">
         <v>133</v>
       </c>
@@ -4146,7 +4146,7 @@
       </c>
     </row>
     <row r="245" spans="1:7">
-      <c r="A245" s="10" t="s">
+      <c r="A245" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B245" s="4"/>
@@ -4161,7 +4161,7 @@
       </c>
     </row>
     <row r="246" spans="1:7">
-      <c r="A246" s="11"/>
+      <c r="A246" s="13"/>
       <c r="B246" s="6" t="s">
         <v>9</v>
       </c>
@@ -4176,7 +4176,7 @@
       </c>
     </row>
     <row r="247" spans="1:7">
-      <c r="A247" s="11"/>
+      <c r="A247" s="13"/>
       <c r="B247" s="7" t="s">
         <v>43</v>
       </c>
@@ -4195,7 +4195,7 @@
       <c r="G247" s="7"/>
     </row>
     <row r="248" spans="1:7" ht="16" thickBot="1">
-      <c r="A248" s="12"/>
+      <c r="A248" s="14"/>
       <c r="B248" s="6" t="s">
         <v>141</v>
       </c>
@@ -4210,7 +4210,7 @@
       </c>
     </row>
     <row r="249" spans="1:7">
-      <c r="A249" s="10" t="s">
+      <c r="A249" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B249" s="4"/>
@@ -4221,7 +4221,7 @@
       <c r="G249" s="4"/>
     </row>
     <row r="250" spans="1:7">
-      <c r="A250" s="11"/>
+      <c r="A250" s="13"/>
       <c r="B250" s="6"/>
       <c r="C250" s="6"/>
       <c r="D250" s="6"/>
@@ -4230,7 +4230,7 @@
       <c r="G250" s="6"/>
     </row>
     <row r="251" spans="1:7">
-      <c r="A251" s="11"/>
+      <c r="A251" s="13"/>
       <c r="B251" s="6" t="s">
         <v>9</v>
       </c>
@@ -4251,7 +4251,7 @@
       </c>
     </row>
     <row r="252" spans="1:7" ht="16" thickBot="1">
-      <c r="A252" s="12"/>
+      <c r="A252" s="14"/>
       <c r="B252" s="8"/>
       <c r="C252" s="8"/>
       <c r="D252" s="8"/>
@@ -4265,19 +4265,19 @@
       </c>
     </row>
     <row r="257" spans="1:7">
-      <c r="A257" s="13"/>
+      <c r="A257" s="11"/>
     </row>
     <row r="258" spans="1:7">
-      <c r="A258" s="13"/>
+      <c r="A258" s="11"/>
     </row>
     <row r="259" spans="1:7" ht="16">
-      <c r="A259" s="13"/>
+      <c r="A259" s="11"/>
       <c r="D259" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:7">
-      <c r="A260" s="13"/>
+      <c r="A260" s="11"/>
     </row>
     <row r="261" spans="1:7">
       <c r="B261" t="s">
@@ -4319,7 +4319,7 @@
       </c>
     </row>
     <row r="265" spans="1:7">
-      <c r="A265" s="10" t="s">
+      <c r="A265" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B265" s="4" t="s">
@@ -4340,7 +4340,7 @@
       </c>
     </row>
     <row r="266" spans="1:7">
-      <c r="A266" s="11"/>
+      <c r="A266" s="13"/>
       <c r="B266" s="6" t="s">
         <v>151</v>
       </c>
@@ -4361,7 +4361,7 @@
       </c>
     </row>
     <row r="267" spans="1:7">
-      <c r="A267" s="11"/>
+      <c r="A267" s="13"/>
       <c r="B267" s="7"/>
       <c r="C267" s="7" t="s">
         <v>154</v>
@@ -4380,7 +4380,7 @@
       </c>
     </row>
     <row r="268" spans="1:7" ht="16" thickBot="1">
-      <c r="A268" s="12"/>
+      <c r="A268" s="14"/>
       <c r="B268" s="6" t="s">
         <v>9</v>
       </c>
@@ -4401,7 +4401,7 @@
       </c>
     </row>
     <row r="269" spans="1:7">
-      <c r="A269" s="10" t="s">
+      <c r="A269" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B269" s="4" t="s">
@@ -4424,7 +4424,7 @@
       </c>
     </row>
     <row r="270" spans="1:7">
-      <c r="A270" s="11"/>
+      <c r="A270" s="13"/>
       <c r="B270" s="6" t="s">
         <v>164</v>
       </c>
@@ -4445,7 +4445,7 @@
       </c>
     </row>
     <row r="271" spans="1:7">
-      <c r="A271" s="11"/>
+      <c r="A271" s="13"/>
       <c r="B271" s="7" t="s">
         <v>149</v>
       </c>
@@ -4466,7 +4466,7 @@
       </c>
     </row>
     <row r="272" spans="1:7" ht="16" thickBot="1">
-      <c r="A272" s="12"/>
+      <c r="A272" s="14"/>
       <c r="B272" s="6" t="s">
         <v>151</v>
       </c>
@@ -4487,7 +4487,7 @@
       </c>
     </row>
     <row r="273" spans="1:7">
-      <c r="A273" s="10" t="s">
+      <c r="A273" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B273" s="4" t="s">
@@ -4504,7 +4504,7 @@
       </c>
     </row>
     <row r="274" spans="1:7">
-      <c r="A274" s="11"/>
+      <c r="A274" s="13"/>
       <c r="B274" s="6" t="s">
         <v>152</v>
       </c>
@@ -4521,7 +4521,7 @@
       </c>
     </row>
     <row r="275" spans="1:7">
-      <c r="A275" s="11"/>
+      <c r="A275" s="13"/>
       <c r="B275" s="7"/>
       <c r="C275" s="7" t="s">
         <v>167</v>
@@ -4540,7 +4540,7 @@
       </c>
     </row>
     <row r="276" spans="1:7" ht="16" thickBot="1">
-      <c r="A276" s="12"/>
+      <c r="A276" s="14"/>
       <c r="B276" s="6" t="s">
         <v>9</v>
       </c>
@@ -4557,7 +4557,7 @@
       </c>
     </row>
     <row r="277" spans="1:7">
-      <c r="A277" s="10" t="s">
+      <c r="A277" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B277" s="4" t="s">
@@ -4574,7 +4574,7 @@
       <c r="G277" s="4"/>
     </row>
     <row r="278" spans="1:7">
-      <c r="A278" s="11"/>
+      <c r="A278" s="13"/>
       <c r="B278" s="6" t="s">
         <v>153</v>
       </c>
@@ -4591,7 +4591,7 @@
       <c r="G278" s="6"/>
     </row>
     <row r="279" spans="1:7">
-      <c r="A279" s="11"/>
+      <c r="A279" s="13"/>
       <c r="B279" s="7" t="s">
         <v>163</v>
       </c>
@@ -4610,7 +4610,7 @@
       </c>
     </row>
     <row r="280" spans="1:7" ht="16" thickBot="1">
-      <c r="A280" s="12"/>
+      <c r="A280" s="14"/>
       <c r="B280" s="6" t="s">
         <v>165</v>
       </c>
@@ -4627,7 +4627,7 @@
       <c r="G280" s="6"/>
     </row>
     <row r="281" spans="1:7">
-      <c r="A281" s="10" t="s">
+      <c r="A281" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B281" s="4"/>
@@ -4644,7 +4644,7 @@
       </c>
     </row>
     <row r="282" spans="1:7">
-      <c r="A282" s="11"/>
+      <c r="A282" s="13"/>
       <c r="B282" s="6" t="s">
         <v>9</v>
       </c>
@@ -4663,7 +4663,7 @@
       </c>
     </row>
     <row r="283" spans="1:7">
-      <c r="A283" s="11"/>
+      <c r="A283" s="13"/>
       <c r="B283" s="7" t="s">
         <v>150</v>
       </c>
@@ -4682,7 +4682,7 @@
       <c r="G283" s="7"/>
     </row>
     <row r="284" spans="1:7" ht="16" thickBot="1">
-      <c r="A284" s="12"/>
+      <c r="A284" s="14"/>
       <c r="B284" s="8" t="s">
         <v>153</v>
       </c>
@@ -4706,19 +4706,19 @@
       </c>
     </row>
     <row r="289" spans="1:7">
-      <c r="A289" s="13"/>
+      <c r="A289" s="11"/>
     </row>
     <row r="290" spans="1:7">
-      <c r="A290" s="13"/>
+      <c r="A290" s="11"/>
     </row>
     <row r="291" spans="1:7" ht="16">
-      <c r="A291" s="13"/>
+      <c r="A291" s="11"/>
       <c r="D291" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="292" spans="1:7">
-      <c r="A292" s="13"/>
+      <c r="A292" s="11"/>
     </row>
     <row r="293" spans="1:7">
       <c r="B293" t="s">
@@ -4760,7 +4760,7 @@
       </c>
     </row>
     <row r="297" spans="1:7">
-      <c r="A297" s="10" t="s">
+      <c r="A297" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B297" s="4"/>
@@ -4773,7 +4773,7 @@
       <c r="G297" s="4"/>
     </row>
     <row r="298" spans="1:7">
-      <c r="A298" s="11"/>
+      <c r="A298" s="13"/>
       <c r="B298" s="6" t="s">
         <v>178</v>
       </c>
@@ -4786,7 +4786,7 @@
       <c r="G298" s="6"/>
     </row>
     <row r="299" spans="1:7">
-      <c r="A299" s="11"/>
+      <c r="A299" s="13"/>
       <c r="B299" s="6" t="s">
         <v>180</v>
       </c>
@@ -4805,7 +4805,7 @@
       </c>
     </row>
     <row r="300" spans="1:7" ht="16" thickBot="1">
-      <c r="A300" s="12"/>
+      <c r="A300" s="14"/>
       <c r="B300" s="6"/>
       <c r="C300" s="6"/>
       <c r="D300" s="6" t="s">
@@ -4816,7 +4816,7 @@
       <c r="G300" s="6"/>
     </row>
     <row r="301" spans="1:7">
-      <c r="A301" s="10" t="s">
+      <c r="A301" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B301" s="4"/>
@@ -4831,7 +4831,7 @@
       </c>
     </row>
     <row r="302" spans="1:7">
-      <c r="A302" s="11"/>
+      <c r="A302" s="13"/>
       <c r="B302" s="6" t="s">
         <v>9</v>
       </c>
@@ -4850,7 +4850,7 @@
       </c>
     </row>
     <row r="303" spans="1:7">
-      <c r="A303" s="11"/>
+      <c r="A303" s="13"/>
       <c r="B303" s="7" t="s">
         <v>161</v>
       </c>
@@ -4869,7 +4869,7 @@
       </c>
     </row>
     <row r="304" spans="1:7" ht="16" thickBot="1">
-      <c r="A304" s="12"/>
+      <c r="A304" s="14"/>
       <c r="B304" s="6" t="s">
         <v>185</v>
       </c>
@@ -4888,7 +4888,7 @@
       </c>
     </row>
     <row r="305" spans="1:7">
-      <c r="A305" s="10" t="s">
+      <c r="A305" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B305" s="4"/>
@@ -4903,7 +4903,7 @@
       <c r="G305" s="4"/>
     </row>
     <row r="306" spans="1:7">
-      <c r="A306" s="11"/>
+      <c r="A306" s="13"/>
       <c r="B306" s="6" t="s">
         <v>9</v>
       </c>
@@ -4922,7 +4922,7 @@
       </c>
     </row>
     <row r="307" spans="1:7">
-      <c r="A307" s="11"/>
+      <c r="A307" s="13"/>
       <c r="B307" s="7" t="s">
         <v>174</v>
       </c>
@@ -4941,7 +4941,7 @@
       </c>
     </row>
     <row r="308" spans="1:7" ht="16" thickBot="1">
-      <c r="A308" s="12"/>
+      <c r="A308" s="14"/>
       <c r="B308" s="6" t="s">
         <v>185</v>
       </c>
@@ -4960,7 +4960,7 @@
       </c>
     </row>
     <row r="309" spans="1:7">
-      <c r="A309" s="10" t="s">
+      <c r="A309" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B309" s="4"/>
@@ -4973,7 +4973,7 @@
       </c>
     </row>
     <row r="310" spans="1:7">
-      <c r="A310" s="11"/>
+      <c r="A310" s="13"/>
       <c r="B310" s="6" t="s">
         <v>9</v>
       </c>
@@ -4988,7 +4988,7 @@
       </c>
     </row>
     <row r="311" spans="1:7">
-      <c r="A311" s="11"/>
+      <c r="A311" s="13"/>
       <c r="B311" s="7" t="s">
         <v>37</v>
       </c>
@@ -5007,7 +5007,7 @@
       <c r="G311" s="7"/>
     </row>
     <row r="312" spans="1:7" ht="16" thickBot="1">
-      <c r="A312" s="12"/>
+      <c r="A312" s="14"/>
       <c r="B312" s="6" t="s">
         <v>180</v>
       </c>
@@ -5022,7 +5022,7 @@
       </c>
     </row>
     <row r="313" spans="1:7">
-      <c r="A313" s="10" t="s">
+      <c r="A313" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B313" s="4"/>
@@ -5035,7 +5035,7 @@
       <c r="G313" s="4"/>
     </row>
     <row r="314" spans="1:7">
-      <c r="A314" s="11"/>
+      <c r="A314" s="13"/>
       <c r="B314" s="6"/>
       <c r="C314" s="6" t="s">
         <v>179</v>
@@ -5048,7 +5048,7 @@
       <c r="G314" s="6"/>
     </row>
     <row r="315" spans="1:7">
-      <c r="A315" s="11"/>
+      <c r="A315" s="13"/>
       <c r="B315" s="6" t="s">
         <v>9</v>
       </c>
@@ -5067,7 +5067,7 @@
       </c>
     </row>
     <row r="316" spans="1:7" ht="16" thickBot="1">
-      <c r="A316" s="12"/>
+      <c r="A316" s="14"/>
       <c r="B316" s="8"/>
       <c r="C316" s="8" t="s">
         <v>9</v>
@@ -5085,19 +5085,19 @@
       </c>
     </row>
     <row r="321" spans="1:7">
-      <c r="A321" s="13"/>
+      <c r="A321" s="11"/>
     </row>
     <row r="322" spans="1:7">
-      <c r="A322" s="13"/>
+      <c r="A322" s="11"/>
     </row>
     <row r="323" spans="1:7" ht="16">
-      <c r="A323" s="13"/>
+      <c r="A323" s="11"/>
       <c r="D323" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:7">
-      <c r="A324" s="13"/>
+      <c r="A324" s="11"/>
     </row>
     <row r="325" spans="1:7">
       <c r="B325" t="s">
@@ -5139,7 +5139,7 @@
       </c>
     </row>
     <row r="329" spans="1:7">
-      <c r="A329" s="10" t="s">
+      <c r="A329" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B329" s="4" t="s">
@@ -5156,7 +5156,7 @@
       <c r="G329" s="4"/>
     </row>
     <row r="330" spans="1:7">
-      <c r="A330" s="11"/>
+      <c r="A330" s="13"/>
       <c r="B330" s="6" t="s">
         <v>194</v>
       </c>
@@ -5173,7 +5173,7 @@
       <c r="G330" s="6"/>
     </row>
     <row r="331" spans="1:7">
-      <c r="A331" s="11"/>
+      <c r="A331" s="13"/>
       <c r="B331" s="7" t="s">
         <v>196</v>
       </c>
@@ -5194,7 +5194,7 @@
       </c>
     </row>
     <row r="332" spans="1:7" ht="16" thickBot="1">
-      <c r="A332" s="12"/>
+      <c r="A332" s="14"/>
       <c r="B332" s="6" t="s">
         <v>199</v>
       </c>
@@ -5211,7 +5211,7 @@
       <c r="G332" s="6"/>
     </row>
     <row r="333" spans="1:7">
-      <c r="A333" s="10" t="s">
+      <c r="A333" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B333" s="4" t="s">
@@ -5228,7 +5228,7 @@
       </c>
     </row>
     <row r="334" spans="1:7">
-      <c r="A334" s="11"/>
+      <c r="A334" s="13"/>
       <c r="B334" s="6" t="s">
         <v>203</v>
       </c>
@@ -5249,7 +5249,7 @@
       </c>
     </row>
     <row r="335" spans="1:7">
-      <c r="A335" s="11"/>
+      <c r="A335" s="13"/>
       <c r="B335" s="7"/>
       <c r="C335" s="7" t="s">
         <v>117</v>
@@ -5266,7 +5266,7 @@
       <c r="G335" s="7"/>
     </row>
     <row r="336" spans="1:7" ht="16" thickBot="1">
-      <c r="A336" s="12"/>
+      <c r="A336" s="14"/>
       <c r="B336" s="6" t="s">
         <v>9</v>
       </c>
@@ -5287,7 +5287,7 @@
       </c>
     </row>
     <row r="337" spans="1:7">
-      <c r="A337" s="10" t="s">
+      <c r="A337" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B337" s="4" t="s">
@@ -5302,7 +5302,7 @@
       <c r="G337" s="4"/>
     </row>
     <row r="338" spans="1:7">
-      <c r="A338" s="11"/>
+      <c r="A338" s="13"/>
       <c r="B338" s="6" t="s">
         <v>206</v>
       </c>
@@ -5317,7 +5317,7 @@
       <c r="G338" s="6"/>
     </row>
     <row r="339" spans="1:7">
-      <c r="A339" s="11"/>
+      <c r="A339" s="13"/>
       <c r="B339" s="7"/>
       <c r="C339" s="7" t="s">
         <v>202</v>
@@ -5334,7 +5334,7 @@
       </c>
     </row>
     <row r="340" spans="1:7" ht="16" thickBot="1">
-      <c r="A340" s="12"/>
+      <c r="A340" s="14"/>
       <c r="B340" s="6" t="s">
         <v>9</v>
       </c>
@@ -5349,7 +5349,7 @@
       <c r="G340" s="6"/>
     </row>
     <row r="341" spans="1:7">
-      <c r="A341" s="10" t="s">
+      <c r="A341" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B341" s="4"/>
@@ -5362,7 +5362,7 @@
       <c r="G341" s="4"/>
     </row>
     <row r="342" spans="1:7">
-      <c r="A342" s="11"/>
+      <c r="A342" s="13"/>
       <c r="B342" s="6"/>
       <c r="C342" s="6"/>
       <c r="D342" s="6" t="s">
@@ -5375,7 +5375,7 @@
       <c r="G342" s="6"/>
     </row>
     <row r="343" spans="1:7">
-      <c r="A343" s="11"/>
+      <c r="A343" s="13"/>
       <c r="B343" s="6" t="s">
         <v>9</v>
       </c>
@@ -5394,7 +5394,7 @@
       </c>
     </row>
     <row r="344" spans="1:7" ht="16" thickBot="1">
-      <c r="A344" s="12"/>
+      <c r="A344" s="14"/>
       <c r="B344" s="6"/>
       <c r="C344" s="6"/>
       <c r="D344" s="6" t="s">
@@ -5407,7 +5407,7 @@
       <c r="G344" s="6"/>
     </row>
     <row r="345" spans="1:7">
-      <c r="A345" s="10" t="s">
+      <c r="A345" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B345" s="4"/>
@@ -5418,7 +5418,7 @@
       <c r="G345" s="4"/>
     </row>
     <row r="346" spans="1:7">
-      <c r="A346" s="11"/>
+      <c r="A346" s="13"/>
       <c r="B346" s="6"/>
       <c r="C346" s="6" t="s">
         <v>9</v>
@@ -5429,7 +5429,7 @@
       <c r="G346" s="6"/>
     </row>
     <row r="347" spans="1:7">
-      <c r="A347" s="11"/>
+      <c r="A347" s="13"/>
       <c r="B347" s="6" t="s">
         <v>9</v>
       </c>
@@ -5450,7 +5450,7 @@
       </c>
     </row>
     <row r="348" spans="1:7" ht="16" thickBot="1">
-      <c r="A348" s="12"/>
+      <c r="A348" s="14"/>
       <c r="B348" s="8"/>
       <c r="C348" s="9" t="s">
         <v>203</v>
@@ -5466,19 +5466,19 @@
       </c>
     </row>
     <row r="353" spans="1:7">
-      <c r="A353" s="13"/>
+      <c r="A353" s="11"/>
     </row>
     <row r="354" spans="1:7">
-      <c r="A354" s="13"/>
+      <c r="A354" s="11"/>
     </row>
     <row r="355" spans="1:7" ht="16">
-      <c r="A355" s="13"/>
+      <c r="A355" s="11"/>
       <c r="D355" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="356" spans="1:7">
-      <c r="A356" s="13"/>
+      <c r="A356" s="11"/>
     </row>
     <row r="357" spans="1:7">
       <c r="B357" t="s">
@@ -5520,7 +5520,7 @@
       </c>
     </row>
     <row r="361" spans="1:7">
-      <c r="A361" s="10" t="s">
+      <c r="A361" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B361" s="4"/>
@@ -5533,7 +5533,7 @@
       <c r="G361" s="4"/>
     </row>
     <row r="362" spans="1:7">
-      <c r="A362" s="11"/>
+      <c r="A362" s="13"/>
       <c r="B362" s="6" t="s">
         <v>9</v>
       </c>
@@ -5546,7 +5546,7 @@
       <c r="G362" s="6"/>
     </row>
     <row r="363" spans="1:7">
-      <c r="A363" s="11"/>
+      <c r="A363" s="13"/>
       <c r="B363" s="7" t="s">
         <v>161</v>
       </c>
@@ -5565,7 +5565,7 @@
       </c>
     </row>
     <row r="364" spans="1:7" ht="16" thickBot="1">
-      <c r="A364" s="12"/>
+      <c r="A364" s="14"/>
       <c r="B364" s="6" t="s">
         <v>213</v>
       </c>
@@ -5578,7 +5578,7 @@
       <c r="G364" s="6"/>
     </row>
     <row r="365" spans="1:7">
-      <c r="A365" s="10" t="s">
+      <c r="A365" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B365" s="4"/>
@@ -5589,7 +5589,7 @@
       <c r="G365" s="4"/>
     </row>
     <row r="366" spans="1:7">
-      <c r="A366" s="11"/>
+      <c r="A366" s="13"/>
       <c r="B366" s="6"/>
       <c r="C366" s="6"/>
       <c r="D366" s="6"/>
@@ -5598,7 +5598,7 @@
       <c r="G366" s="6"/>
     </row>
     <row r="367" spans="1:7">
-      <c r="A367" s="11"/>
+      <c r="A367" s="13"/>
       <c r="B367" s="6" t="s">
         <v>9</v>
       </c>
@@ -5619,7 +5619,7 @@
       </c>
     </row>
     <row r="368" spans="1:7" ht="16" thickBot="1">
-      <c r="A368" s="12"/>
+      <c r="A368" s="14"/>
       <c r="B368" s="6"/>
       <c r="C368" s="6"/>
       <c r="D368" s="6"/>
@@ -5628,7 +5628,7 @@
       <c r="G368" s="6"/>
     </row>
     <row r="369" spans="1:7">
-      <c r="A369" s="10" t="s">
+      <c r="A369" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B369" s="4" t="s">
@@ -5641,7 +5641,7 @@
       <c r="G369" s="4"/>
     </row>
     <row r="370" spans="1:7">
-      <c r="A370" s="11"/>
+      <c r="A370" s="13"/>
       <c r="B370" s="6" t="s">
         <v>213</v>
       </c>
@@ -5652,7 +5652,7 @@
       <c r="G370" s="6"/>
     </row>
     <row r="371" spans="1:7">
-      <c r="A371" s="11"/>
+      <c r="A371" s="13"/>
       <c r="B371" s="7"/>
       <c r="C371" s="6" t="s">
         <v>9</v>
@@ -5671,7 +5671,7 @@
       </c>
     </row>
     <row r="372" spans="1:7" ht="16" thickBot="1">
-      <c r="A372" s="12"/>
+      <c r="A372" s="14"/>
       <c r="B372" s="6" t="s">
         <v>9</v>
       </c>
@@ -5682,7 +5682,7 @@
       <c r="G372" s="6"/>
     </row>
     <row r="373" spans="1:7">
-      <c r="A373" s="10" t="s">
+      <c r="A373" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B373" s="4"/>
@@ -5693,7 +5693,7 @@
       <c r="G373" s="4"/>
     </row>
     <row r="374" spans="1:7">
-      <c r="A374" s="11"/>
+      <c r="A374" s="13"/>
       <c r="B374" s="6"/>
       <c r="C374" s="6"/>
       <c r="D374" s="6" t="s">
@@ -5704,7 +5704,7 @@
       <c r="G374" s="6"/>
     </row>
     <row r="375" spans="1:7">
-      <c r="A375" s="11"/>
+      <c r="A375" s="13"/>
       <c r="B375" s="6" t="s">
         <v>9</v>
       </c>
@@ -5725,7 +5725,7 @@
       </c>
     </row>
     <row r="376" spans="1:7" ht="16" thickBot="1">
-      <c r="A376" s="12"/>
+      <c r="A376" s="14"/>
       <c r="B376" s="6"/>
       <c r="C376" s="6"/>
       <c r="D376" s="6" t="s">
@@ -5736,7 +5736,7 @@
       <c r="G376" s="6"/>
     </row>
     <row r="377" spans="1:7">
-      <c r="A377" s="10" t="s">
+      <c r="A377" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B377" s="4"/>
@@ -5747,7 +5747,7 @@
       <c r="G377" s="4"/>
     </row>
     <row r="378" spans="1:7">
-      <c r="A378" s="11"/>
+      <c r="A378" s="13"/>
       <c r="B378" s="6"/>
       <c r="C378" s="6"/>
       <c r="D378" s="6"/>
@@ -5756,7 +5756,7 @@
       <c r="G378" s="6"/>
     </row>
     <row r="379" spans="1:7">
-      <c r="A379" s="11"/>
+      <c r="A379" s="13"/>
       <c r="B379" s="6" t="s">
         <v>9</v>
       </c>
@@ -5777,7 +5777,7 @@
       </c>
     </row>
     <row r="380" spans="1:7" ht="16" thickBot="1">
-      <c r="A380" s="12"/>
+      <c r="A380" s="14"/>
       <c r="B380" s="8"/>
       <c r="C380" s="8"/>
       <c r="D380" s="8"/>
@@ -5791,19 +5791,19 @@
       </c>
     </row>
     <row r="385" spans="1:7">
-      <c r="A385" s="13"/>
+      <c r="A385" s="11"/>
     </row>
     <row r="386" spans="1:7">
-      <c r="A386" s="13"/>
+      <c r="A386" s="11"/>
     </row>
     <row r="387" spans="1:7" ht="16">
-      <c r="A387" s="13"/>
+      <c r="A387" s="11"/>
       <c r="D387" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="388" spans="1:7">
-      <c r="A388" s="13"/>
+      <c r="A388" s="11"/>
     </row>
     <row r="389" spans="1:7">
       <c r="B389" t="s">
@@ -5845,7 +5845,7 @@
       </c>
     </row>
     <row r="393" spans="1:7">
-      <c r="A393" s="10" t="s">
+      <c r="A393" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B393" s="4"/>
@@ -5866,7 +5866,7 @@
       </c>
     </row>
     <row r="394" spans="1:7">
-      <c r="A394" s="11"/>
+      <c r="A394" s="13"/>
       <c r="B394" s="6" t="s">
         <v>9</v>
       </c>
@@ -5887,7 +5887,7 @@
       </c>
     </row>
     <row r="395" spans="1:7">
-      <c r="A395" s="11"/>
+      <c r="A395" s="13"/>
       <c r="B395" s="7" t="s">
         <v>222</v>
       </c>
@@ -5906,7 +5906,7 @@
       </c>
     </row>
     <row r="396" spans="1:7" ht="16" thickBot="1">
-      <c r="A396" s="12"/>
+      <c r="A396" s="14"/>
       <c r="B396" s="6" t="s">
         <v>225</v>
       </c>
@@ -5927,7 +5927,7 @@
       </c>
     </row>
     <row r="397" spans="1:7">
-      <c r="A397" s="10" t="s">
+      <c r="A397" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B397" s="4" t="s">
@@ -5950,7 +5950,7 @@
       </c>
     </row>
     <row r="398" spans="1:7">
-      <c r="A398" s="11"/>
+      <c r="A398" s="13"/>
       <c r="B398" s="6" t="s">
         <v>225</v>
       </c>
@@ -5971,7 +5971,7 @@
       </c>
     </row>
     <row r="399" spans="1:7">
-      <c r="A399" s="11"/>
+      <c r="A399" s="13"/>
       <c r="B399" s="7" t="s">
         <v>236</v>
       </c>
@@ -5992,7 +5992,7 @@
       </c>
     </row>
     <row r="400" spans="1:7" ht="16" thickBot="1">
-      <c r="A400" s="12"/>
+      <c r="A400" s="14"/>
       <c r="B400" s="6" t="s">
         <v>233</v>
       </c>
@@ -6013,7 +6013,7 @@
       </c>
     </row>
     <row r="401" spans="1:7">
-      <c r="A401" s="10" t="s">
+      <c r="A401" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B401" s="4" t="s">
@@ -6036,7 +6036,7 @@
       </c>
     </row>
     <row r="402" spans="1:7">
-      <c r="A402" s="11"/>
+      <c r="A402" s="13"/>
       <c r="B402" s="6" t="s">
         <v>241</v>
       </c>
@@ -6057,7 +6057,7 @@
       </c>
     </row>
     <row r="403" spans="1:7">
-      <c r="A403" s="11"/>
+      <c r="A403" s="13"/>
       <c r="B403" s="7" t="s">
         <v>244</v>
       </c>
@@ -6076,7 +6076,7 @@
       </c>
     </row>
     <row r="404" spans="1:7" ht="16" thickBot="1">
-      <c r="A404" s="12"/>
+      <c r="A404" s="14"/>
       <c r="B404" s="6" t="s">
         <v>217</v>
       </c>
@@ -6097,7 +6097,7 @@
       </c>
     </row>
     <row r="405" spans="1:7">
-      <c r="A405" s="10" t="s">
+      <c r="A405" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B405" s="4"/>
@@ -6116,7 +6116,7 @@
       </c>
     </row>
     <row r="406" spans="1:7">
-      <c r="A406" s="11"/>
+      <c r="A406" s="13"/>
       <c r="B406" s="6" t="s">
         <v>9</v>
       </c>
@@ -6135,7 +6135,7 @@
       </c>
     </row>
     <row r="407" spans="1:7">
-      <c r="A407" s="11"/>
+      <c r="A407" s="13"/>
       <c r="B407" s="7" t="s">
         <v>223</v>
       </c>
@@ -6156,7 +6156,7 @@
       </c>
     </row>
     <row r="408" spans="1:7" ht="16" thickBot="1">
-      <c r="A408" s="12"/>
+      <c r="A408" s="14"/>
       <c r="B408" s="6" t="s">
         <v>232</v>
       </c>
@@ -6175,7 +6175,7 @@
       </c>
     </row>
     <row r="409" spans="1:7">
-      <c r="A409" s="10" t="s">
+      <c r="A409" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B409" s="4"/>
@@ -6192,7 +6192,7 @@
       <c r="G409" s="4"/>
     </row>
     <row r="410" spans="1:7">
-      <c r="A410" s="11"/>
+      <c r="A410" s="13"/>
       <c r="B410" s="6" t="s">
         <v>9</v>
       </c>
@@ -6209,7 +6209,7 @@
       <c r="G410" s="6"/>
     </row>
     <row r="411" spans="1:7">
-      <c r="A411" s="11"/>
+      <c r="A411" s="13"/>
       <c r="B411" s="7" t="s">
         <v>122</v>
       </c>
@@ -6230,7 +6230,7 @@
       </c>
     </row>
     <row r="412" spans="1:7" ht="16" thickBot="1">
-      <c r="A412" s="12"/>
+      <c r="A412" s="14"/>
       <c r="B412" s="8" t="s">
         <v>242</v>
       </c>
@@ -6252,19 +6252,19 @@
       </c>
     </row>
     <row r="417" spans="1:7">
-      <c r="A417" s="13"/>
+      <c r="A417" s="11"/>
     </row>
     <row r="418" spans="1:7">
-      <c r="A418" s="13"/>
+      <c r="A418" s="11"/>
     </row>
     <row r="419" spans="1:7" ht="16">
-      <c r="A419" s="13"/>
+      <c r="A419" s="11"/>
       <c r="D419" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="420" spans="1:7">
-      <c r="A420" s="13"/>
+      <c r="A420" s="11"/>
     </row>
     <row r="421" spans="1:7">
       <c r="B421" t="s">
@@ -6306,7 +6306,7 @@
       </c>
     </row>
     <row r="425" spans="1:7">
-      <c r="A425" s="10" t="s">
+      <c r="A425" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B425" s="4" t="s">
@@ -6321,7 +6321,7 @@
       <c r="G425" s="4"/>
     </row>
     <row r="426" spans="1:7">
-      <c r="A426" s="11"/>
+      <c r="A426" s="13"/>
       <c r="B426" s="6" t="s">
         <v>15</v>
       </c>
@@ -6342,7 +6342,7 @@
       </c>
     </row>
     <row r="427" spans="1:7">
-      <c r="A427" s="11"/>
+      <c r="A427" s="13"/>
       <c r="B427" s="7"/>
       <c r="C427" s="7" t="s">
         <v>161</v>
@@ -6361,7 +6361,7 @@
       </c>
     </row>
     <row r="428" spans="1:7" ht="16" thickBot="1">
-      <c r="A428" s="12"/>
+      <c r="A428" s="14"/>
       <c r="B428" s="6" t="s">
         <v>9</v>
       </c>
@@ -6382,7 +6382,7 @@
       </c>
     </row>
     <row r="429" spans="1:7">
-      <c r="A429" s="10" t="s">
+      <c r="A429" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B429" s="4" t="s">
@@ -6403,7 +6403,7 @@
       </c>
     </row>
     <row r="430" spans="1:7">
-      <c r="A430" s="11"/>
+      <c r="A430" s="13"/>
       <c r="B430" s="6" t="s">
         <v>213</v>
       </c>
@@ -6424,7 +6424,7 @@
       </c>
     </row>
     <row r="431" spans="1:7">
-      <c r="A431" s="11"/>
+      <c r="A431" s="13"/>
       <c r="B431" s="7" t="s">
         <v>47</v>
       </c>
@@ -6441,7 +6441,7 @@
       <c r="G431" s="7"/>
     </row>
     <row r="432" spans="1:7" ht="16" thickBot="1">
-      <c r="A432" s="12"/>
+      <c r="A432" s="14"/>
       <c r="B432" s="6" t="s">
         <v>262</v>
       </c>
@@ -6462,7 +6462,7 @@
       </c>
     </row>
     <row r="433" spans="1:7">
-      <c r="A433" s="10" t="s">
+      <c r="A433" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B433" s="4" t="s">
@@ -6481,7 +6481,7 @@
       </c>
     </row>
     <row r="434" spans="1:7">
-      <c r="A434" s="11"/>
+      <c r="A434" s="13"/>
       <c r="B434" s="6" t="s">
         <v>213</v>
       </c>
@@ -6500,7 +6500,7 @@
       </c>
     </row>
     <row r="435" spans="1:7">
-      <c r="A435" s="11"/>
+      <c r="A435" s="13"/>
       <c r="B435" s="7"/>
       <c r="C435" s="7" t="s">
         <v>116</v>
@@ -6519,7 +6519,7 @@
       </c>
     </row>
     <row r="436" spans="1:7" ht="16" thickBot="1">
-      <c r="A436" s="12"/>
+      <c r="A436" s="14"/>
       <c r="B436" s="6" t="s">
         <v>9</v>
       </c>
@@ -6538,7 +6538,7 @@
       </c>
     </row>
     <row r="437" spans="1:7">
-      <c r="A437" s="10" t="s">
+      <c r="A437" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B437" s="4"/>
@@ -6557,7 +6557,7 @@
       </c>
     </row>
     <row r="438" spans="1:7">
-      <c r="A438" s="11"/>
+      <c r="A438" s="13"/>
       <c r="B438" s="6" t="s">
         <v>9</v>
       </c>
@@ -6578,7 +6578,7 @@
       </c>
     </row>
     <row r="439" spans="1:7">
-      <c r="A439" s="11"/>
+      <c r="A439" s="13"/>
       <c r="B439" s="7" t="s">
         <v>269</v>
       </c>
@@ -6597,7 +6597,7 @@
       </c>
     </row>
     <row r="440" spans="1:7" ht="16" thickBot="1">
-      <c r="A440" s="12"/>
+      <c r="A440" s="14"/>
       <c r="B440" s="6" t="s">
         <v>254</v>
       </c>
@@ -6618,7 +6618,7 @@
       </c>
     </row>
     <row r="441" spans="1:7">
-      <c r="A441" s="10" t="s">
+      <c r="A441" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B441" s="4" t="s">
@@ -6637,7 +6637,7 @@
       <c r="G441" s="4"/>
     </row>
     <row r="442" spans="1:7">
-      <c r="A442" s="11"/>
+      <c r="A442" s="13"/>
       <c r="B442" s="6" t="s">
         <v>274</v>
       </c>
@@ -6654,7 +6654,7 @@
       <c r="G442" s="6"/>
     </row>
     <row r="443" spans="1:7">
-      <c r="A443" s="11"/>
+      <c r="A443" s="13"/>
       <c r="B443" s="7" t="s">
         <v>272</v>
       </c>
@@ -6673,7 +6673,7 @@
       </c>
     </row>
     <row r="444" spans="1:7" ht="16" thickBot="1">
-      <c r="A444" s="12"/>
+      <c r="A444" s="14"/>
       <c r="B444" s="8" t="s">
         <v>15</v>
       </c>
@@ -6695,19 +6695,19 @@
       </c>
     </row>
     <row r="449" spans="1:7">
-      <c r="A449" s="13"/>
+      <c r="A449" s="11"/>
     </row>
     <row r="450" spans="1:7">
-      <c r="A450" s="13"/>
+      <c r="A450" s="11"/>
     </row>
     <row r="451" spans="1:7" ht="16">
-      <c r="A451" s="13"/>
+      <c r="A451" s="11"/>
       <c r="D451" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="452" spans="1:7">
-      <c r="A452" s="13"/>
+      <c r="A452" s="11"/>
     </row>
     <row r="453" spans="1:7">
       <c r="B453" t="s">
@@ -6749,7 +6749,7 @@
       </c>
     </row>
     <row r="457" spans="1:7">
-      <c r="A457" s="10" t="s">
+      <c r="A457" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B457" s="4"/>
@@ -6760,7 +6760,7 @@
       <c r="G457" s="4"/>
     </row>
     <row r="458" spans="1:7">
-      <c r="A458" s="11"/>
+      <c r="A458" s="13"/>
       <c r="B458" s="6" t="s">
         <v>9</v>
       </c>
@@ -6771,7 +6771,7 @@
       <c r="G458" s="6"/>
     </row>
     <row r="459" spans="1:7">
-      <c r="A459" s="11"/>
+      <c r="A459" s="13"/>
       <c r="B459" s="7" t="s">
         <v>175</v>
       </c>
@@ -6792,7 +6792,7 @@
       </c>
     </row>
     <row r="460" spans="1:7" ht="16" thickBot="1">
-      <c r="A460" s="12"/>
+      <c r="A460" s="14"/>
       <c r="B460" s="6" t="s">
         <v>238</v>
       </c>
@@ -6803,7 +6803,7 @@
       <c r="G460" s="6"/>
     </row>
     <row r="461" spans="1:7">
-      <c r="A461" s="10" t="s">
+      <c r="A461" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B461" s="4"/>
@@ -6816,7 +6816,7 @@
       <c r="G461" s="4"/>
     </row>
     <row r="462" spans="1:7">
-      <c r="A462" s="11"/>
+      <c r="A462" s="13"/>
       <c r="B462" s="6" t="s">
         <v>9</v>
       </c>
@@ -6829,7 +6829,7 @@
       <c r="G462" s="6"/>
     </row>
     <row r="463" spans="1:7">
-      <c r="A463" s="11"/>
+      <c r="A463" s="13"/>
       <c r="B463" s="7" t="s">
         <v>276</v>
       </c>
@@ -6848,7 +6848,7 @@
       </c>
     </row>
     <row r="464" spans="1:7" ht="16" thickBot="1">
-      <c r="A464" s="12"/>
+      <c r="A464" s="14"/>
       <c r="B464" s="6" t="s">
         <v>277</v>
       </c>
@@ -6861,7 +6861,7 @@
       <c r="G464" s="6"/>
     </row>
     <row r="465" spans="1:7">
-      <c r="A465" s="10" t="s">
+      <c r="A465" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B465" s="4"/>
@@ -6878,7 +6878,7 @@
       </c>
     </row>
     <row r="466" spans="1:7">
-      <c r="A466" s="11"/>
+      <c r="A466" s="13"/>
       <c r="B466" s="6"/>
       <c r="C466" s="6" t="s">
         <v>280</v>
@@ -6895,7 +6895,7 @@
       </c>
     </row>
     <row r="467" spans="1:7">
-      <c r="A467" s="11"/>
+      <c r="A467" s="13"/>
       <c r="B467" s="6" t="s">
         <v>9</v>
       </c>
@@ -6912,7 +6912,7 @@
       <c r="G467" s="7"/>
     </row>
     <row r="468" spans="1:7" ht="16" thickBot="1">
-      <c r="A468" s="12"/>
+      <c r="A468" s="14"/>
       <c r="B468" s="6"/>
       <c r="C468" s="6" t="s">
         <v>9</v>
@@ -6927,7 +6927,7 @@
       </c>
     </row>
     <row r="469" spans="1:7">
-      <c r="A469" s="10" t="s">
+      <c r="A469" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B469" s="4" t="s">
@@ -6946,7 +6946,7 @@
       </c>
     </row>
     <row r="470" spans="1:7">
-      <c r="A470" s="11"/>
+      <c r="A470" s="13"/>
       <c r="B470" s="6" t="s">
         <v>280</v>
       </c>
@@ -6963,7 +6963,7 @@
       </c>
     </row>
     <row r="471" spans="1:7">
-      <c r="A471" s="11"/>
+      <c r="A471" s="13"/>
       <c r="B471" s="7"/>
       <c r="C471" s="6" t="s">
         <v>9</v>
@@ -6982,7 +6982,7 @@
       </c>
     </row>
     <row r="472" spans="1:7" ht="16" thickBot="1">
-      <c r="A472" s="12"/>
+      <c r="A472" s="14"/>
       <c r="B472" s="6" t="s">
         <v>9</v>
       </c>
@@ -6999,7 +6999,7 @@
       </c>
     </row>
     <row r="473" spans="1:7">
-      <c r="A473" s="10" t="s">
+      <c r="A473" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B473" s="4"/>
@@ -7010,7 +7010,7 @@
       <c r="G473" s="4"/>
     </row>
     <row r="474" spans="1:7">
-      <c r="A474" s="11"/>
+      <c r="A474" s="13"/>
       <c r="B474" s="6"/>
       <c r="C474" s="6"/>
       <c r="D474" s="6" t="s">
@@ -7021,7 +7021,7 @@
       <c r="G474" s="6"/>
     </row>
     <row r="475" spans="1:7">
-      <c r="A475" s="11"/>
+      <c r="A475" s="13"/>
       <c r="B475" s="6" t="s">
         <v>9</v>
       </c>
@@ -7042,7 +7042,7 @@
       </c>
     </row>
     <row r="476" spans="1:7" ht="16" thickBot="1">
-      <c r="A476" s="12"/>
+      <c r="A476" s="14"/>
       <c r="B476" s="8"/>
       <c r="C476" s="8"/>
       <c r="D476" s="8" t="s">
@@ -7059,12 +7059,74 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A461:A464"/>
+    <mergeCell ref="A465:A468"/>
+    <mergeCell ref="A469:A472"/>
+    <mergeCell ref="A473:A476"/>
+    <mergeCell ref="A437:A440"/>
+    <mergeCell ref="A441:A444"/>
+    <mergeCell ref="A449:A452"/>
+    <mergeCell ref="A457:A460"/>
+    <mergeCell ref="A417:A420"/>
+    <mergeCell ref="A425:A428"/>
+    <mergeCell ref="A429:A432"/>
+    <mergeCell ref="A433:A436"/>
+    <mergeCell ref="A397:A400"/>
+    <mergeCell ref="A401:A404"/>
+    <mergeCell ref="A405:A408"/>
+    <mergeCell ref="A409:A412"/>
+    <mergeCell ref="A373:A376"/>
+    <mergeCell ref="A377:A380"/>
+    <mergeCell ref="A385:A388"/>
+    <mergeCell ref="A393:A396"/>
+    <mergeCell ref="A353:A356"/>
+    <mergeCell ref="A361:A364"/>
+    <mergeCell ref="A365:A368"/>
+    <mergeCell ref="A369:A372"/>
+    <mergeCell ref="A333:A336"/>
+    <mergeCell ref="A337:A340"/>
+    <mergeCell ref="A341:A344"/>
+    <mergeCell ref="A345:A348"/>
+    <mergeCell ref="A309:A312"/>
+    <mergeCell ref="A313:A316"/>
+    <mergeCell ref="A321:A324"/>
+    <mergeCell ref="A329:A332"/>
+    <mergeCell ref="A289:A292"/>
+    <mergeCell ref="A297:A300"/>
+    <mergeCell ref="A301:A304"/>
+    <mergeCell ref="A305:A308"/>
+    <mergeCell ref="A269:A272"/>
+    <mergeCell ref="A273:A276"/>
+    <mergeCell ref="A277:A280"/>
+    <mergeCell ref="A281:A284"/>
+    <mergeCell ref="A245:A248"/>
+    <mergeCell ref="A249:A252"/>
+    <mergeCell ref="A257:A260"/>
+    <mergeCell ref="A265:A268"/>
+    <mergeCell ref="A225:A228"/>
+    <mergeCell ref="A233:A236"/>
+    <mergeCell ref="A237:A240"/>
+    <mergeCell ref="A241:A244"/>
+    <mergeCell ref="A217:A220"/>
+    <mergeCell ref="A193:A196"/>
+    <mergeCell ref="A201:A204"/>
+    <mergeCell ref="A205:A208"/>
+    <mergeCell ref="A209:A212"/>
+    <mergeCell ref="A213:A216"/>
+    <mergeCell ref="A173:A176"/>
+    <mergeCell ref="A177:A180"/>
+    <mergeCell ref="A185:A188"/>
+    <mergeCell ref="A129:A132"/>
+    <mergeCell ref="A153:A156"/>
+    <mergeCell ref="A161:A164"/>
+    <mergeCell ref="A181:A184"/>
+    <mergeCell ref="A169:A172"/>
+    <mergeCell ref="A149:A152"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="A109:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="A137:A140"/>
+    <mergeCell ref="A141:A144"/>
     <mergeCell ref="A33:A36"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="A45:A48"/>
@@ -7081,74 +7143,12 @@
     <mergeCell ref="A81:A84"/>
     <mergeCell ref="A85:A88"/>
     <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="A109:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="A137:A140"/>
-    <mergeCell ref="A141:A144"/>
-    <mergeCell ref="A173:A176"/>
-    <mergeCell ref="A177:A180"/>
-    <mergeCell ref="A185:A188"/>
-    <mergeCell ref="A129:A132"/>
-    <mergeCell ref="A153:A156"/>
-    <mergeCell ref="A161:A164"/>
-    <mergeCell ref="A181:A184"/>
-    <mergeCell ref="A169:A172"/>
-    <mergeCell ref="A149:A152"/>
-    <mergeCell ref="A217:A220"/>
-    <mergeCell ref="A193:A196"/>
-    <mergeCell ref="A201:A204"/>
-    <mergeCell ref="A205:A208"/>
-    <mergeCell ref="A209:A212"/>
-    <mergeCell ref="A213:A216"/>
-    <mergeCell ref="A245:A248"/>
-    <mergeCell ref="A249:A252"/>
-    <mergeCell ref="A257:A260"/>
-    <mergeCell ref="A265:A268"/>
-    <mergeCell ref="A225:A228"/>
-    <mergeCell ref="A233:A236"/>
-    <mergeCell ref="A237:A240"/>
-    <mergeCell ref="A241:A244"/>
-    <mergeCell ref="A289:A292"/>
-    <mergeCell ref="A297:A300"/>
-    <mergeCell ref="A301:A304"/>
-    <mergeCell ref="A305:A308"/>
-    <mergeCell ref="A269:A272"/>
-    <mergeCell ref="A273:A276"/>
-    <mergeCell ref="A277:A280"/>
-    <mergeCell ref="A281:A284"/>
-    <mergeCell ref="A333:A336"/>
-    <mergeCell ref="A337:A340"/>
-    <mergeCell ref="A341:A344"/>
-    <mergeCell ref="A345:A348"/>
-    <mergeCell ref="A309:A312"/>
-    <mergeCell ref="A313:A316"/>
-    <mergeCell ref="A321:A324"/>
-    <mergeCell ref="A329:A332"/>
-    <mergeCell ref="A373:A376"/>
-    <mergeCell ref="A377:A380"/>
-    <mergeCell ref="A385:A388"/>
-    <mergeCell ref="A393:A396"/>
-    <mergeCell ref="A353:A356"/>
-    <mergeCell ref="A361:A364"/>
-    <mergeCell ref="A365:A368"/>
-    <mergeCell ref="A369:A372"/>
-    <mergeCell ref="A417:A420"/>
-    <mergeCell ref="A425:A428"/>
-    <mergeCell ref="A429:A432"/>
-    <mergeCell ref="A433:A436"/>
-    <mergeCell ref="A397:A400"/>
-    <mergeCell ref="A401:A404"/>
-    <mergeCell ref="A405:A408"/>
-    <mergeCell ref="A409:A412"/>
-    <mergeCell ref="A461:A464"/>
-    <mergeCell ref="A465:A468"/>
-    <mergeCell ref="A469:A472"/>
-    <mergeCell ref="A473:A476"/>
-    <mergeCell ref="A437:A440"/>
-    <mergeCell ref="A441:A444"/>
-    <mergeCell ref="A449:A452"/>
-    <mergeCell ref="A457:A460"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A21:A24"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>